<commit_message>
updates to inventory JG
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariana/Desktop/historical_tech/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennagreene/historical_tech/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B66A94-5497-FD44-A432-93CD71E0D467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F81504-B0E2-4C4E-90DC-6B8B0E5B9506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1000" windowWidth="28420" windowHeight="15760" activeTab="1" xr2:uid="{27AF86FA-D4C6-8648-9C3F-13CEB56E391C}"/>
+    <workbookView xWindow="180" yWindow="500" windowWidth="14280" windowHeight="15760" activeTab="1" xr2:uid="{27AF86FA-D4C6-8648-9C3F-13CEB56E391C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="208">
   <si>
     <t>Refineries</t>
   </si>
@@ -637,6 +637,30 @@
   </si>
   <si>
     <t>Data Source</t>
+  </si>
+  <si>
+    <t>Ideas JG</t>
+  </si>
+  <si>
+    <t>CHAT database (radio)</t>
+  </si>
+  <si>
+    <t>CHAT database, from Mitchell (railline)</t>
+  </si>
+  <si>
+    <t>CHAT database, from Mitchell (ship_steam)</t>
+  </si>
+  <si>
+    <t>CHAT database, from Mitchell and World Bank (telephone)</t>
+  </si>
+  <si>
+    <t>CHAT database, from Banks and World Bank (tv)</t>
+  </si>
+  <si>
+    <t>CHAT database, from Mitchell and World Bank (vehicle_car, might also include vehicle_com?)</t>
+  </si>
+  <si>
+    <t>Might be mostly US focused</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28CB4A72-1B50-8C4D-B6E7-06C4748F18B9}">
   <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A69" sqref="A1:A69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2185,177 +2209,189 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436B7163-F664-2046-84C9-DED64B10C419}">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>198</v>
       </c>
       <c r="B1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>159</v>
       </c>
@@ -2440,114 +2476,138 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <f>COUNTA(B2:B70)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <f>B71/69</f>
+        <v>8.6956521739130432E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>